<commit_message>
2번째 lastIndexOf && 주석 추가
</commit_message>
<xml_diff>
--- a/isbn.xlsx
+++ b/isbn.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>책제목</t>
   </si>
@@ -41,25 +41,13 @@
     <t>도우출판</t>
   </si>
   <si>
-    <t xml:space="preserve"> 리눅스 프로그래밍</t>
-  </si>
-  <si>
-    <t>창병모</t>
-  </si>
-  <si>
-    <t>생능출판</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>9788994492032</t>
   </si>
   <si>
-    <t>hello.jpg</t>
-  </si>
-  <si>
-    <t>9791156645580</t>
+    <t>20230207163634.jpg</t>
   </si>
 </sst>
 </file>
@@ -142,50 +130,12 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1333500" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -225,30 +175,12 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F2"/>
-    </row>
-    <row r="3" ht="120.0" customHeight="true">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
fix:FileOutputStream fileName bug fixgit add .
</commit_message>
<xml_diff>
--- a/isbn.xlsx
+++ b/isbn.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>책제목</t>
   </si>
@@ -41,13 +41,28 @@
     <t>도우출판</t>
   </si>
   <si>
+    <t>리눅스 프로그래밍</t>
+  </si>
+  <si>
+    <t>창병모</t>
+  </si>
+  <si>
+    <t>생능출판</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
     <t>9788994492032</t>
   </si>
   <si>
-    <t>20230207163634.jpg</t>
+    <t xml:space="preserve">20230207163634.jpg     </t>
+  </si>
+  <si>
+    <t>9791156007968</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20230117163158.jpg     </t>
   </si>
 </sst>
 </file>
@@ -130,12 +145,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1333500" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -175,12 +228,30 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2"/>
+    </row>
+    <row r="3" ht="120.0" customHeight="true">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="F2"/>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>